<commit_message>
updated results and plots
</commit_message>
<xml_diff>
--- a/experiments/2023_05_stress_pose_scientific_reports/results/overview_features.xlsx
+++ b/experiments/2023_05_stress_pose_scientific_reports/results/overview_features.xlsx
@@ -406,13 +406,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C2">
         <v>390</v>
       </c>
       <c r="D2">
-        <v>479</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -444,13 +444,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>365</v>
       </c>
       <c r="D2">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>